<commit_message>
New results from importance of storage pool, and various parameter settings
New results from importance of storage pool, temperature and plant size
dependant parameter settings, varying a set of parameters (not all at a
time) for different treatments
</commit_message>
<xml_diff>
--- a/archieve/compare_parameter_settings/Compare_parameter_settings.xlsx
+++ b/archieve/compare_parameter_settings/Compare_parameter_settings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10400" yWindow="4000" windowWidth="28000" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="-27900" yWindow="3920" windowWidth="27860" windowHeight="14080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>BIC (Combined)</t>
   </si>
@@ -35,31 +35,46 @@
     <t>Case #</t>
   </si>
   <si>
-    <t>All parameters different</t>
-  </si>
-  <si>
-    <t>Allocations constant</t>
-  </si>
-  <si>
-    <t>k and Y constant</t>
-  </si>
-  <si>
-    <t>Turnovers constant</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>Parameter settings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Works equally well as case 1, except the roots </t>
-  </si>
-  <si>
-    <t>All parameters constant</t>
-  </si>
-  <si>
     <t>Doesn’t fit the data well enough</t>
+  </si>
+  <si>
+    <t>All parameters different - time depandant</t>
+  </si>
+  <si>
+    <t>All parameters constant - time depandant</t>
+  </si>
+  <si>
+    <t>k and Y constant - time depandant</t>
+  </si>
+  <si>
+    <t>Allocations constant - time depandant</t>
+  </si>
+  <si>
+    <t>Turnovers constant - time depandant</t>
+  </si>
+  <si>
+    <t>All parameters different - temperature depandant</t>
+  </si>
+  <si>
+    <t>All parameters different - plant size (height) depandant</t>
+  </si>
+  <si>
+    <t>The model needs the storage pool</t>
+  </si>
+  <si>
+    <t>All parameters different - No storage pool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Works equally well as case 2, except the roots </t>
+  </si>
+  <si>
+    <t>Parameter settings (Linear variation)</t>
+  </si>
+  <si>
+    <t>Linear variation has the best data fit</t>
   </si>
 </sst>
 </file>
@@ -388,18 +403,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="28.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="49.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -408,13 +423,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -422,10 +437,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1373</v>
+        <v>12</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1507</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -433,13 +451,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1">
-        <v>3240</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1373</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -447,10 +465,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
-        <v>1420</v>
+        <v>3240</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -458,13 +479,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
-        <v>1392</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -472,10 +490,52 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
+        <v>1392</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
         <v>1416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1433</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1514</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Considering NSC partitioning uncertainty
Include the NSC partitioning uncertainty into the model simulation for
WTC3 as I did for GPP and respiration components
</commit_message>
<xml_diff>
--- a/archieve/compare_parameter_settings/Compare_parameter_settings.xlsx
+++ b/archieve/compare_parameter_settings/Compare_parameter_settings.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>BIC (Combined)</t>
   </si>
@@ -38,43 +38,46 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Doesn’t fit the data well enough</t>
-  </si>
-  <si>
-    <t>All parameters different - time depandant</t>
-  </si>
-  <si>
-    <t>All parameters constant - time depandant</t>
-  </si>
-  <si>
-    <t>k and Y constant - time depandant</t>
-  </si>
-  <si>
-    <t>Allocations constant - time depandant</t>
-  </si>
-  <si>
-    <t>Turnovers constant - time depandant</t>
-  </si>
-  <si>
-    <t>All parameters different - temperature depandant</t>
-  </si>
-  <si>
-    <t>All parameters different - plant size (height) depandant</t>
-  </si>
-  <si>
     <t>The model needs the storage pool</t>
   </si>
   <si>
     <t>All parameters different - No storage pool</t>
   </si>
   <si>
-    <t xml:space="preserve">Works equally well as case 2, except the roots </t>
-  </si>
-  <si>
     <t>Parameter settings (Linear variation)</t>
   </si>
   <si>
     <t>Linear variation has the best data fit</t>
+  </si>
+  <si>
+    <t>There is certain effect of warming on parameters</t>
+  </si>
+  <si>
+    <t>Works slightly worse than case 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Works almost equally well as case 2, except the roots </t>
+  </si>
+  <si>
+    <t>All parameters different - time dependent</t>
+  </si>
+  <si>
+    <t>All parameters constant - time dependent</t>
+  </si>
+  <si>
+    <t>k and Y constant - time dependent</t>
+  </si>
+  <si>
+    <t>Allocations constant - time dependent</t>
+  </si>
+  <si>
+    <t>Turnovers constant - time dependent</t>
+  </si>
+  <si>
+    <t>All parameters different - temperature dependent</t>
+  </si>
+  <si>
+    <t>All parameters different - plant size (height) dependent</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -414,7 +417,7 @@
     <col min="1" max="1" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="49.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -423,7 +426,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -437,13 +440,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1">
         <v>1507</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -451,13 +454,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2">
         <v>1373</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -465,13 +468,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>3240</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -479,10 +482,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>1420</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -490,13 +496,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1">
         <v>1392</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -504,10 +510,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1">
         <v>1416</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -515,13 +524,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1">
         <v>1433</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -529,13 +538,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1">
         <v>1514</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>